<commit_message>
Added Return ticket functionality and experimented with data driven testing, fixing null values
</commit_message>
<xml_diff>
--- a/TrainBooking/src/test/resources/data/data.xlsx
+++ b/TrainBooking/src/test/resources/data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
   <si>
     <t>From</t>
   </si>
@@ -49,19 +49,25 @@
     <t>30</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>London Bridge</t>
   </si>
   <si>
     <t>Waterloo</t>
   </si>
   <si>
-    <t>21/08/2022</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>22/04/2022</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -72,8 +78,8 @@
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -86,6 +92,104 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -100,38 +204,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,69 +218,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,14 +228,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,181 +249,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,9 +439,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,30 +472,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -490,17 +483,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,8 +505,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,142 +539,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1064,28 +1070,28 @@
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>